<commit_message>
Refactor package data loading to use DataHashingUtils
</commit_message>
<xml_diff>
--- a/data/WGUPS Distance Table.xlsx
+++ b/data/WGUPS Distance Table.xlsx
@@ -253,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +270,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -564,43 +570,43 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -618,7 +624,7 @@
     <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1770,7 +1776,7 @@
       <c r="AB18" s="27"/>
       <c r="AC18" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="23.7">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="27">
       <c r="A19" s="24" t="s">
         <v>13</v>
       </c>
@@ -1827,7 +1833,7 @@
       <c r="AB19" s="27"/>
       <c r="AC19" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="23.7">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="27">
       <c r="A20" s="24" t="s">
         <v>14</v>
       </c>
@@ -1886,7 +1892,7 @@
       <c r="AB20" s="27"/>
       <c r="AC20" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="23.7">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="27">
       <c r="A21" s="24" t="s">
         <v>15</v>
       </c>
@@ -1947,7 +1953,7 @@
       <c r="AB21" s="27"/>
       <c r="AC21" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="23.7">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="27">
       <c r="A22" s="24" t="s">
         <v>16</v>
       </c>
@@ -2010,7 +2016,7 @@
       <c r="AB22" s="27"/>
       <c r="AC22" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="36">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="37.5">
       <c r="A23" s="24" t="s">
         <v>17</v>
       </c>
@@ -2075,7 +2081,7 @@
       <c r="AB23" s="27"/>
       <c r="AC23" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="36">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="37.5">
       <c r="A24" s="24" t="s">
         <v>18</v>
       </c>
@@ -2142,7 +2148,7 @@
       <c r="AB24" s="27"/>
       <c r="AC24" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="48">
       <c r="A25" s="24" t="s">
         <v>19</v>
       </c>
@@ -2211,7 +2217,7 @@
       <c r="AB25" s="27"/>
       <c r="AC25" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="37.5">
       <c r="A26" s="24" t="s">
         <v>20</v>
       </c>
@@ -2282,7 +2288,7 @@
       <c r="AB26" s="27"/>
       <c r="AC26" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="37.5">
       <c r="A27" s="24" t="s">
         <v>21</v>
       </c>
@@ -2355,7 +2361,7 @@
       <c r="AB27" s="27"/>
       <c r="AC27" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="23.7">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="37.5">
       <c r="A28" s="24" t="s">
         <v>22</v>
       </c>
@@ -2430,7 +2436,7 @@
       <c r="AB28" s="27"/>
       <c r="AC28" s="28"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="37.5">
       <c r="A29" s="24" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Refactor data parsing logic to handle empty cells and symmetric values
</commit_message>
<xml_diff>
--- a/data/WGUPS Distance Table.xlsx
+++ b/data/WGUPS Distance Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>WGUPS Distance Table</t>
   </si>
@@ -142,8 +142,16 @@
     <t xml:space="preserve"> HUB</t>
   </si>
   <si>
+    <t>International Peace Gardens
+ 1060 Dalton Ave S</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 1060 Dalton Ave S
 (84104)</t>
+  </si>
+  <si>
+    <t>Sugar House Park
+ 1330 2100 S</t>
   </si>
   <si>
     <t xml:space="preserve"> 1330 2100 S
@@ -1355,10 +1363,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="37.5">
       <c r="A10" s="24" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="25">
         <v>7.2</v>
@@ -1394,10 +1402,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="27">
       <c r="A11" s="24" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="25">
         <v>3.8</v>
@@ -1438,7 +1446,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="25">
         <v>11</v>
@@ -1481,7 +1489,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" s="25">
         <v>2.2</v>
@@ -1526,7 +1534,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="25">
         <v>3.5</v>
@@ -1573,7 +1581,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C15" s="25">
         <v>10.9</v>
@@ -1622,7 +1630,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" s="25">
         <v>8.6</v>
@@ -1673,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="25">
         <v>7.6</v>
@@ -1726,7 +1734,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C18" s="25">
         <v>2.8</v>
@@ -1781,7 +1789,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19" s="25">
         <v>6.4</v>
@@ -1838,7 +1846,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C20" s="25">
         <v>3.2</v>
@@ -1897,7 +1905,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="25">
         <v>7.6</v>
@@ -1958,7 +1966,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="25">
         <v>5.2</v>
@@ -2021,7 +2029,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C23" s="25">
         <v>4.4</v>
@@ -2086,7 +2094,7 @@
         <v>18</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24" s="25">
         <v>3.66112816434</v>
@@ -2153,7 +2161,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C25" s="25">
         <v>7.6</v>
@@ -2222,7 +2230,7 @@
         <v>20</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C26" s="25">
         <v>2</v>
@@ -2293,7 +2301,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C27" s="25">
         <v>3.6</v>
@@ -2366,7 +2374,7 @@
         <v>22</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C28" s="25">
         <v>6.5</v>
@@ -2441,7 +2449,7 @@
         <v>23</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C29" s="25">
         <v>1.9</v>
@@ -2518,7 +2526,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C30" s="25">
         <v>3.4</v>
@@ -2597,7 +2605,7 @@
         <v>25</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="25">
         <v>2.4</v>
@@ -2678,7 +2686,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C32" s="25">
         <v>6.4</v>
@@ -2761,7 +2769,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C33" s="25">
         <v>2.4</v>
@@ -2846,7 +2854,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C34" s="25">
         <v>5</v>
@@ -2933,7 +2941,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C35" s="30">
         <v>3.6</v>

</xml_diff>